<commit_message>
correção do interceptor e do toast
</commit_message>
<xml_diff>
--- a/src/assets/files/exemplo_local.xlsx
+++ b/src/assets/files/exemplo_local.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Planilha1!$A$1:$J$418</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Planilha1!$A$1:$J$418</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,11 +23,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">nome</t>
   </si>
   <si>
+    <t xml:space="preserve">descrição</t>
+  </si>
+  <si>
     <t xml:space="preserve">nome_responsável</t>
   </si>
   <si>
@@ -35,6 +38,63 @@
   </si>
   <si>
     <t xml:space="preserve">telefone_responsável</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nome 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setor 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">responsavel setor 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">responsavel_setor1@electroson.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F000006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nome 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setor 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">responsavel setor 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">responsavel_setor2@elecroson.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F000011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nome 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setor 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">responsavel setor 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">responsavel_setor3@electroson.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F000013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F000015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F000025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F000027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F000029</t>
   </si>
 </sst>
 </file>
@@ -149,10 +209,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -160,57 +216,137 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="49.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="41.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.15"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>111111111</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>222222222</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>333333333</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J418"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="responsavel_setor1@electroson.com"/>
+    <hyperlink ref="E3" r:id="rId2" display="responsavel_setor2@elecroson.com"/>
+    <hyperlink ref="E4" r:id="rId3" display="responsavel_setor3@electroson.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>